<commit_message>
feature/backend: 12500 알람 예외 처리, HIM, DCM 버전 정보 추가
</commit_message>
<xml_diff>
--- a/apps/conveyor/backend/log-troller/sbin/R301.xlsx
+++ b/apps/conveyor/backend/log-troller/sbin/R301.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/works/semi-ts/conveyor/monorepo/apps/conveyor/backend/sbin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimmy/works/semi-ts/conveyor/monorepo/apps/conveyor/backend/log-troller/sbin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BA8598-5569-2F49-8E95-00DF4693429B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF9FECE-93FE-3A4D-BFAE-B62B07D8E531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51720" yWindow="500" windowWidth="32360" windowHeight="25340" tabRatio="812" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36440" yWindow="500" windowWidth="32360" windowHeight="25340" tabRatio="812" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Domain" sheetId="1" r:id="rId1"/>
@@ -1262,7 +1262,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1333,6 +1333,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1391,7 +1399,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1442,6 +1450,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1730,7 +1741,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -2581,7 +2592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -5510,7 +5521,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -6140,8 +6151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
@@ -6207,8 +6218,8 @@
       <c r="A3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>22</v>
+      <c r="B3" s="18" t="s">
+        <v>128</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>14</v>

</xml_diff>